<commit_message>
updated Alco Corp ticker from AA US to 7777666D US
</commit_message>
<xml_diff>
--- a/company_data/sample/M&A List A-S&P500 T-US Sample Set.xlsx
+++ b/company_data/sample/M&A List A-S&P500 T-US Sample Set.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="445">
   <si>
     <t>Deal Type</t>
   </si>
@@ -1367,6 +1367,9 @@
   </si>
   <si>
     <t>Also have PX_HIGH, PX_LOW, and PX_MID</t>
+  </si>
+  <si>
+    <t>7777666D US</t>
   </si>
 </sst>
 </file>
@@ -5306,8 +5309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5316,6 +5319,7 @@
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -7722,7 +7726,7 @@
         <v>338</v>
       </c>
       <c r="H55" t="s">
-        <v>339</v>
+        <v>444</v>
       </c>
       <c r="I55" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
minor tweeks to the file
</commit_message>
<xml_diff>
--- a/company_data/sample/M&A List A-S&P500 T-US Sample Set.xlsx
+++ b/company_data/sample/M&A List A-S&P500 T-US Sample Set.xlsx
@@ -5309,9 +5309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9368,7 +9366,7 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>